<commit_message>
Minutes of the meeting added
</commit_message>
<xml_diff>
--- a/Phase 2/Meeting Tracker.xlsx
+++ b/Phase 2/Meeting Tracker.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/81bf44df4e7f0b96/Documents/GitHub/CMPG-315/Phase 2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{271B8554-E63C-443D-ABAB-0ED02868BCB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="60" documentId="8_{271B8554-E63C-443D-ABAB-0ED02868BCB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{827421D4-3F77-4F67-80A6-C97CBEE2EE2F}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{274A3E9E-9E00-4E6D-B64C-6C85BF5F9384}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{274A3E9E-9E00-4E6D-B64C-6C85BF5F9384}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Meetings" sheetId="1" r:id="rId1"/>
+    <sheet name="1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,9 +36,74 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
+  <si>
+    <t>Column2</t>
+  </si>
+  <si>
+    <t>Column3</t>
+  </si>
+  <si>
+    <t>Column4</t>
+  </si>
+  <si>
+    <t>Column5</t>
+  </si>
+  <si>
+    <t>Mariska</t>
+  </si>
+  <si>
+    <t>Lia</t>
+  </si>
+  <si>
+    <t>Ethan</t>
+  </si>
+  <si>
+    <t>Marnus</t>
+  </si>
+  <si>
+    <t>Christoffel</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>13:00 - 14:00</t>
+  </si>
+  <si>
+    <t>MEETING TRACKER</t>
+  </si>
+  <si>
+    <t>Meeting 1 : Minutes of the meeting</t>
+  </si>
+  <si>
+    <t>Mariska is appointed as leader</t>
+  </si>
+  <si>
+    <t>What we are expected to do is discussed</t>
+  </si>
+  <si>
+    <t>We got to know each other</t>
+  </si>
+  <si>
+    <t>We appointed the work to do (due 8 April)</t>
+  </si>
+  <si>
+    <t>We allso made a discord server for future meeting since the semester week is close</t>
+  </si>
+  <si>
+    <t>We made a googlde drive document for our first phase</t>
+  </si>
+  <si>
+    <t>Everyone familiarized themselves with the github project/repository Mariska made beforehand</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -45,16 +111,53 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="26"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -62,17 +165,89 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -83,6 +258,20 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A17C1F39-E364-4212-8E96-F9197E3A878F}" name="Table1" displayName="Table1" ref="B5:F10" totalsRowShown="0" dataDxfId="0">
+  <autoFilter ref="B5:F10" xr:uid="{A17C1F39-E364-4212-8E96-F9197E3A878F}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{09C91160-9D3B-403C-A3A3-01BE9EF0C1E5}" name="13:00 - 14:00" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{E35E6BAE-EB84-4E5D-B700-A276AA20C593}" name="Column2" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{5E8A74E9-D380-4F9D-B7F7-F30BDAFF04F6}" name="Column3" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{8295A03C-03F8-4E74-B483-F14DABA65EC6}" name="Column4" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{4360DE7A-184E-46FA-B55F-5DEF2A5AFADE}" name="Column5" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -402,12 +591,179 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36B31534-06A3-4BF3-8B8F-0E1862B0C6B3}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="10.33203125" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="10.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A1" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="7"/>
+      <c r="B4" s="6">
+        <v>45748</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="8"/>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4068502-E0A7-48A9-9691-818782A343CB}">
+  <dimension ref="A1:A9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S8" sqref="S8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A1" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated minutes of the meeting
</commit_message>
<xml_diff>
--- a/Phase 2/Meeting Tracker.xlsx
+++ b/Phase 2/Meeting Tracker.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/81bf44df4e7f0b96/Documents/GitHub/CMPG-315/Phase 2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="82" documentId="8_{271B8554-E63C-443D-ABAB-0ED02868BCB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{350E49E1-3FD3-4171-8544-F9400E68E901}"/>
+  <xr:revisionPtr revIDLastSave="94" documentId="8_{271B8554-E63C-443D-ABAB-0ED02868BCB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9CEC03E0-C9A6-4840-BE37-6A7BA34EA1BD}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{274A3E9E-9E00-4E6D-B64C-6C85BF5F9384}"/>
+    <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{274A3E9E-9E00-4E6D-B64C-6C85BF5F9384}"/>
   </bookViews>
   <sheets>
     <sheet name="Meetings" sheetId="1" r:id="rId1"/>
     <sheet name="1" sheetId="2" r:id="rId2"/>
     <sheet name="2" sheetId="3" r:id="rId3"/>
+    <sheet name="3" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
   <si>
     <t>Column3</t>
   </si>
@@ -122,6 +123,30 @@
   </si>
   <si>
     <t>Ethan and Christoffel - Machine room</t>
+  </si>
+  <si>
+    <t>Meeting 3: Minutes of the meeting</t>
+  </si>
+  <si>
+    <t>Discussed what technologies to use for the chatapp</t>
+  </si>
+  <si>
+    <t>Desided on using python</t>
+  </si>
+  <si>
+    <t>Chatted about all outstanding documentation to be done</t>
+  </si>
+  <si>
+    <t>Discussed merging all the documentation already done into one document</t>
+  </si>
+  <si>
+    <t>Discussed making a powerpoint presentation for the demo day</t>
+  </si>
+  <si>
+    <t>Discussed having a "work day/s" on the weekend</t>
+  </si>
+  <si>
+    <t>Planned a work day on Saterday between 10 and 5</t>
   </si>
 </sst>
 </file>
@@ -284,10 +309,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -810,9 +831,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0CEAEE8-BB1C-43FA-BC9E-97052DFBE2A6}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -859,4 +878,59 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34A97F62-973D-409B-B172-BE38EBC21ACE}">
+  <dimension ref="A1:A8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A1" s="10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>